<commit_message>
committing new update to raw
</commit_message>
<xml_diff>
--- a/data/Meyer_nrec2023decompbagdata.xlsx
+++ b/data/Meyer_nrec2023decompbagdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RyanMeyer/Documents/R Projects/2023_nrec_decomp/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wlperry/Documents/r_projects/NREC_Decomp_2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD56E32C-C40B-8C4A-8347-D9FD0903E77D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849C4CD4-7F1C-164E-9787-31EC807166CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15660" xr2:uid="{4A753238-9247-8848-863F-14539E74CA07}"/>
+    <workbookView xWindow="1060" yWindow="760" windowWidth="28800" windowHeight="15660" xr2:uid="{4A753238-9247-8848-863F-14539E74CA07}"/>
   </bookViews>
   <sheets>
     <sheet name="compressed" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2703" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2704" uniqueCount="529">
   <si>
     <t>id</t>
   </si>
@@ -1621,6 +1621,9 @@
   </si>
   <si>
     <t>tea bag ripped</t>
+  </si>
+  <si>
+    <t>notes</t>
   </si>
 </sst>
 </file>
@@ -1986,8 +1989,8 @@
   <dimension ref="A1:Q401"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O5" sqref="O5"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2053,6 +2056,9 @@
       </c>
       <c r="P1" t="s">
         <v>502</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>528</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Cleaning and importing data.
</commit_message>
<xml_diff>
--- a/data/Meyer_nrec2023decompbagdata.xlsx
+++ b/data/Meyer_nrec2023decompbagdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wlperry/Documents/r_projects/NREC_Decomp_2/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RyanMeyer/Documents/R Projects/2023_nrec_decomp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849C4CD4-7F1C-164E-9787-31EC807166CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7CBC3B-5F61-A644-A6AB-80C1789A6AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="760" windowWidth="28800" windowHeight="15660" xr2:uid="{4A753238-9247-8848-863F-14539E74CA07}"/>
+    <workbookView xWindow="0" yWindow="520" windowWidth="28800" windowHeight="15660" xr2:uid="{4A753238-9247-8848-863F-14539E74CA07}"/>
   </bookViews>
   <sheets>
     <sheet name="compressed" sheetId="2" r:id="rId1"/>
@@ -1989,8 +1989,8 @@
   <dimension ref="A1:Q401"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
+      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M213" sqref="M213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11926,9 +11926,13 @@
         <v>18.196999999999999</v>
       </c>
       <c r="M205">
+        <f t="shared" si="7"/>
+        <v>18.096999999999998</v>
+      </c>
+      <c r="N205">
         <v>205</v>
       </c>
-      <c r="N205">
+      <c r="O205">
         <v>1.1619999999999999</v>
       </c>
     </row>
@@ -12825,9 +12829,13 @@
         <v>9.8040000000000003</v>
       </c>
       <c r="M224">
+        <f>L224-I229</f>
+        <v>9.7040000000000006</v>
+      </c>
+      <c r="N224">
         <v>222</v>
       </c>
-      <c r="N224">
+      <c r="O224">
         <v>1.4650000000000001</v>
       </c>
     </row>

</xml_diff>